<commit_message>
Additions to Resource list.  Changes in blogdown library and changes to theme CSS to support floating code folding button
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10909"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerhardgroenewald/Documents/R Projects/gerhardgroenewald.co.uk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{32DAC944-106F-3446-AB29-F22C26071C7F}" xr6:coauthVersionLast="37" xr6:coauthVersionMax="37" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C23DF4-22A7-A742-8997-02FBB64C8B26}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="28800" windowHeight="18000" xr2:uid="{D09C6361-AE78-2141-8FAE-67D4DAF24799}"/>
+    <workbookView xWindow="33360" yWindow="440" windowWidth="28800" windowHeight="18000" xr2:uid="{D09C6361-AE78-2141-8FAE-67D4DAF24799}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="376" uniqueCount="194">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="200">
   <si>
     <t>Source</t>
   </si>
@@ -609,6 +609,24 @@
   </si>
   <si>
     <t>https://scholar.google.com/citations?user=W9CxPFIAAAAJ&amp;hl=en</t>
+  </si>
+  <si>
+    <t>Essence of Linear Algebra</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLZHQObOWTQDPD3MizzM2xVFitgF8hE_ab</t>
+  </si>
+  <si>
+    <t>Grant Sanderson</t>
+  </si>
+  <si>
+    <t>https://www.3blue1brown.com/about/</t>
+  </si>
+  <si>
+    <t>Essence of Calculus</t>
+  </si>
+  <si>
+    <t>https://www.youtube.com/playlist?list=PLZHQObOWTQDMsr9K-rj53DwVRMYO3t5Yr</t>
   </si>
 </sst>
 </file>
@@ -974,10 +992,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275A2A9A-7374-FC4C-AFC4-53788431EF74}">
-  <dimension ref="A1:I43"/>
+  <dimension ref="A1:I45"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A24" zoomScale="129" workbookViewId="0">
-      <selection activeCell="B39" sqref="B39"/>
+    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="129" workbookViewId="0">
+      <selection activeCell="B45" sqref="B45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1994,6 +2012,52 @@
       </c>
       <c r="H43" s="2" t="s">
         <v>143</v>
+      </c>
+    </row>
+    <row r="44" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>7</v>
+      </c>
+      <c r="B44" t="s">
+        <v>9</v>
+      </c>
+      <c r="C44" t="s">
+        <v>108</v>
+      </c>
+      <c r="D44" t="s">
+        <v>120</v>
+      </c>
+      <c r="F44" t="s">
+        <v>194</v>
+      </c>
+      <c r="G44" t="s">
+        <v>196</v>
+      </c>
+      <c r="H44" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="45" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>7</v>
+      </c>
+      <c r="B45" t="s">
+        <v>115</v>
+      </c>
+      <c r="C45" t="s">
+        <v>108</v>
+      </c>
+      <c r="D45" t="s">
+        <v>120</v>
+      </c>
+      <c r="F45" t="s">
+        <v>198</v>
+      </c>
+      <c r="G45" t="s">
+        <v>196</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>199</v>
       </c>
     </row>
   </sheetData>
@@ -2040,6 +2104,8 @@
     <hyperlink ref="H41" r:id="rId40" xr:uid="{9E383B6C-6E2B-0B4A-9920-A2A2592A4E93}"/>
     <hyperlink ref="H42" r:id="rId41" xr:uid="{AEAC8E0D-36A7-F74C-9A98-3F00555A6C56}"/>
     <hyperlink ref="H43" r:id="rId42" xr:uid="{EA1B315E-C585-884A-9D4B-458B01F703F0}"/>
+    <hyperlink ref="H44" r:id="rId43" xr:uid="{69BD5659-0F20-614B-9C4F-3A61021D6A98}"/>
+    <hyperlink ref="H45" r:id="rId44" xr:uid="{9E13235A-1E25-8145-BE2D-EA8A78F0F883}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2048,10 +2114,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6A4CF0-E7B1-A149-8123-B7914F3BFAC3}">
-  <dimension ref="A1:B33"/>
+  <dimension ref="A1:B34"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B13" sqref="B13"/>
+      <selection activeCell="A34" sqref="A34"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2324,7 +2390,18 @@
         <v>193</v>
       </c>
     </row>
+    <row r="34" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A34" t="s">
+        <v>196</v>
+      </c>
+      <c r="B34" s="2" t="s">
+        <v>197</v>
+      </c>
+    </row>
   </sheetData>
+  <hyperlinks>
+    <hyperlink ref="B34" r:id="rId1" xr:uid="{EB0E88FC-9F49-F04E-BD45-78B47D7913D3}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>

</xml_diff>

<commit_message>
update with Resume, updated Resource, and About
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="11208"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerhardgroenewald/Documents/R Projects/gerhardgroenewald.co.uk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{71C23DF4-22A7-A742-8997-02FBB64C8B26}" xr6:coauthVersionLast="40" xr6:coauthVersionMax="40" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAE5C90-7616-AF4C-A731-92251FD46DFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="33360" yWindow="440" windowWidth="28800" windowHeight="18000" xr2:uid="{D09C6361-AE78-2141-8FAE-67D4DAF24799}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D09C6361-AE78-2141-8FAE-67D4DAF24799}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="392" uniqueCount="200">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="209">
   <si>
     <t>Source</t>
   </si>
@@ -627,6 +627,33 @@
   </si>
   <si>
     <t>https://www.youtube.com/playlist?list=PLZHQObOWTQDMsr9K-rj53DwVRMYO3t5Yr</t>
+  </si>
+  <si>
+    <t>https://geocompr.robinlovelace.net</t>
+  </si>
+  <si>
+    <t>Geocomputation with R</t>
+  </si>
+  <si>
+    <t>Robin Lovelace, Jakub Nowosad, Jannes Muenchow</t>
+  </si>
+  <si>
+    <t>https://www.robinlovelace.net</t>
+  </si>
+  <si>
+    <t>Robin Lovelace</t>
+  </si>
+  <si>
+    <t>https://nowosad.github.io</t>
+  </si>
+  <si>
+    <t>Jakub Nowosad</t>
+  </si>
+  <si>
+    <t>Jannes Muenchow</t>
+  </si>
+  <si>
+    <t>https://www.geographie.uni-jena.de/en/Muenchow.html</t>
   </si>
 </sst>
 </file>
@@ -992,10 +1019,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275A2A9A-7374-FC4C-AFC4-53788431EF74}">
-  <dimension ref="A1:I45"/>
+  <dimension ref="A1:I47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A20" zoomScale="129" workbookViewId="0">
-      <selection activeCell="B45" sqref="B45"/>
+    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
+      <selection activeCell="C3" sqref="C3:H3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -1036,7 +1063,7 @@
         <v>38</v>
       </c>
     </row>
-    <row r="2" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>7</v>
       </c>
@@ -1044,73 +1071,73 @@
         <v>26</v>
       </c>
       <c r="C2" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D2" t="s">
         <v>6</v>
       </c>
       <c r="F2" t="s">
-        <v>4</v>
-      </c>
-      <c r="G2" s="1" t="s">
-        <v>17</v>
+        <v>201</v>
+      </c>
+      <c r="G2" t="s">
+        <v>202</v>
       </c>
       <c r="H2" s="2" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="3" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="3" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B3" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C3" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D3" t="s">
         <v>6</v>
       </c>
       <c r="F3" t="s">
-        <v>40</v>
-      </c>
-      <c r="G3" s="1" t="s">
+        <v>201</v>
+      </c>
+      <c r="G3" t="s">
+        <v>202</v>
+      </c>
+      <c r="H3" s="2" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="4" spans="1:9" ht="17" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>7</v>
+      </c>
+      <c r="B4" t="s">
+        <v>26</v>
+      </c>
+      <c r="C4" t="s">
+        <v>108</v>
+      </c>
+      <c r="D4" t="s">
+        <v>6</v>
+      </c>
+      <c r="F4" t="s">
+        <v>4</v>
+      </c>
+      <c r="G4" s="1" t="s">
         <v>17</v>
       </c>
-      <c r="H3" s="2" t="s">
-        <v>41</v>
-      </c>
-    </row>
-    <row r="4" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>8</v>
-      </c>
-      <c r="B4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C4" t="s">
-        <v>108</v>
-      </c>
-      <c r="D4" t="s">
-        <v>120</v>
-      </c>
-      <c r="F4" t="s">
-        <v>11</v>
-      </c>
-      <c r="G4" t="s">
-        <v>12</v>
-      </c>
       <c r="H4" s="2" t="s">
-        <v>10</v>
-      </c>
-    </row>
-    <row r="5" spans="1:9" x14ac:dyDescent="0.2">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="5" spans="1:9" ht="17" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>8</v>
       </c>
       <c r="B5" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C5" t="s">
         <v>108</v>
@@ -1119,13 +1146,13 @@
         <v>6</v>
       </c>
       <c r="F5" t="s">
-        <v>15</v>
-      </c>
-      <c r="G5" t="s">
-        <v>16</v>
+        <v>40</v>
+      </c>
+      <c r="G5" s="1" t="s">
+        <v>17</v>
       </c>
       <c r="H5" s="2" t="s">
-        <v>21</v>
+        <v>41</v>
       </c>
     </row>
     <row r="6" spans="1:9" x14ac:dyDescent="0.2">
@@ -1133,22 +1160,22 @@
         <v>8</v>
       </c>
       <c r="B6" t="s">
-        <v>26</v>
+        <v>9</v>
       </c>
       <c r="C6" t="s">
         <v>108</v>
       </c>
       <c r="D6" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="F6" t="s">
-        <v>18</v>
+        <v>11</v>
       </c>
       <c r="G6" t="s">
-        <v>20</v>
+        <v>12</v>
       </c>
       <c r="H6" s="2" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
     </row>
     <row r="7" spans="1:9" x14ac:dyDescent="0.2">
@@ -1156,7 +1183,7 @@
         <v>8</v>
       </c>
       <c r="B7" t="s">
-        <v>105</v>
+        <v>14</v>
       </c>
       <c r="C7" t="s">
         <v>108</v>
@@ -1165,62 +1192,59 @@
         <v>6</v>
       </c>
       <c r="F7" t="s">
-        <v>23</v>
+        <v>15</v>
       </c>
       <c r="G7" t="s">
-        <v>24</v>
+        <v>16</v>
       </c>
       <c r="H7" s="2" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
     </row>
     <row r="8" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B8" t="s">
-        <v>105</v>
+        <v>26</v>
       </c>
       <c r="C8" t="s">
         <v>108</v>
       </c>
       <c r="D8" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F8" t="s">
-        <v>33</v>
+        <v>18</v>
       </c>
       <c r="G8" t="s">
-        <v>34</v>
+        <v>20</v>
       </c>
       <c r="H8" s="2" t="s">
-        <v>109</v>
+        <v>19</v>
       </c>
     </row>
     <row r="9" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B9" t="s">
-        <v>26</v>
+        <v>105</v>
       </c>
       <c r="C9" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D9" t="s">
         <v>6</v>
       </c>
-      <c r="E9" t="s">
-        <v>28</v>
-      </c>
       <c r="F9" t="s">
-        <v>28</v>
+        <v>23</v>
       </c>
       <c r="G9" t="s">
-        <v>29</v>
+        <v>24</v>
       </c>
       <c r="H9" s="2" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
     </row>
     <row r="10" spans="1:9" x14ac:dyDescent="0.2">
@@ -1228,45 +1252,48 @@
         <v>7</v>
       </c>
       <c r="B10" t="s">
-        <v>121</v>
+        <v>105</v>
       </c>
       <c r="C10" t="s">
         <v>108</v>
       </c>
       <c r="D10" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="F10" t="s">
-        <v>32</v>
+        <v>33</v>
       </c>
       <c r="G10" t="s">
-        <v>31</v>
+        <v>34</v>
       </c>
       <c r="H10" s="2" t="s">
-        <v>30</v>
+        <v>109</v>
       </c>
     </row>
     <row r="11" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B11" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="C11" t="s">
-        <v>123</v>
+        <v>122</v>
       </c>
       <c r="D11" t="s">
         <v>6</v>
       </c>
+      <c r="E11" t="s">
+        <v>28</v>
+      </c>
       <c r="F11" t="s">
-        <v>35</v>
+        <v>28</v>
       </c>
       <c r="G11" t="s">
-        <v>36</v>
+        <v>29</v>
       </c>
       <c r="H11" s="2" t="s">
-        <v>37</v>
+        <v>27</v>
       </c>
     </row>
     <row r="12" spans="1:9" x14ac:dyDescent="0.2">
@@ -1274,22 +1301,22 @@
         <v>7</v>
       </c>
       <c r="B12" t="s">
-        <v>106</v>
+        <v>121</v>
       </c>
       <c r="C12" t="s">
         <v>108</v>
       </c>
       <c r="D12" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="F12" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="G12" t="s">
-        <v>36</v>
+        <v>31</v>
       </c>
       <c r="H12" s="2" t="s">
-        <v>39</v>
+        <v>30</v>
       </c>
     </row>
     <row r="13" spans="1:9" x14ac:dyDescent="0.2">
@@ -1300,88 +1327,88 @@
         <v>106</v>
       </c>
       <c r="C13" t="s">
-        <v>108</v>
+        <v>123</v>
       </c>
       <c r="D13" t="s">
         <v>6</v>
       </c>
       <c r="F13" t="s">
-        <v>42</v>
+        <v>35</v>
       </c>
       <c r="G13" t="s">
-        <v>44</v>
+        <v>36</v>
       </c>
       <c r="H13" s="2" t="s">
-        <v>43</v>
+        <v>37</v>
       </c>
     </row>
     <row r="14" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
-        <v>45</v>
+        <v>7</v>
       </c>
       <c r="B14" t="s">
-        <v>105</v>
+        <v>106</v>
       </c>
       <c r="C14" t="s">
         <v>108</v>
       </c>
       <c r="D14" t="s">
-        <v>60</v>
+        <v>6</v>
       </c>
       <c r="F14" t="s">
-        <v>48</v>
+        <v>35</v>
       </c>
       <c r="G14" t="s">
-        <v>47</v>
+        <v>36</v>
       </c>
       <c r="H14" s="2" t="s">
-        <v>46</v>
+        <v>39</v>
       </c>
     </row>
     <row r="15" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B15" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="C15" t="s">
         <v>108</v>
       </c>
       <c r="D15" t="s">
-        <v>22</v>
+        <v>6</v>
       </c>
       <c r="F15" t="s">
-        <v>53</v>
+        <v>42</v>
       </c>
       <c r="G15" t="s">
-        <v>51</v>
+        <v>44</v>
       </c>
       <c r="H15" s="2" t="s">
-        <v>49</v>
+        <v>43</v>
       </c>
     </row>
     <row r="16" spans="1:9" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
-        <v>7</v>
+        <v>45</v>
       </c>
       <c r="B16" t="s">
-        <v>106</v>
+        <v>105</v>
       </c>
       <c r="C16" t="s">
         <v>108</v>
       </c>
       <c r="D16" t="s">
-        <v>22</v>
+        <v>60</v>
       </c>
       <c r="F16" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="G16" t="s">
-        <v>51</v>
+        <v>47</v>
       </c>
       <c r="H16" s="2" t="s">
-        <v>52</v>
+        <v>46</v>
       </c>
     </row>
     <row r="17" spans="1:8" x14ac:dyDescent="0.2">
@@ -1398,13 +1425,13 @@
         <v>22</v>
       </c>
       <c r="F17" t="s">
-        <v>59</v>
+        <v>53</v>
       </c>
       <c r="G17" t="s">
         <v>51</v>
       </c>
       <c r="H17" s="2" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
     </row>
     <row r="18" spans="1:8" x14ac:dyDescent="0.2">
@@ -1412,7 +1439,7 @@
         <v>7</v>
       </c>
       <c r="B18" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="C18" t="s">
         <v>108</v>
@@ -1421,13 +1448,13 @@
         <v>22</v>
       </c>
       <c r="F18" t="s">
-        <v>62</v>
+        <v>50</v>
       </c>
       <c r="G18" t="s">
-        <v>104</v>
+        <v>51</v>
       </c>
       <c r="H18" s="2" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
     </row>
     <row r="19" spans="1:8" x14ac:dyDescent="0.2">
@@ -1435,7 +1462,7 @@
         <v>7</v>
       </c>
       <c r="B19" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="C19" t="s">
         <v>108</v>
@@ -1444,13 +1471,13 @@
         <v>22</v>
       </c>
       <c r="F19" t="s">
-        <v>64</v>
+        <v>59</v>
       </c>
       <c r="G19" t="s">
-        <v>65</v>
+        <v>51</v>
       </c>
       <c r="H19" s="2" t="s">
-        <v>63</v>
+        <v>58</v>
       </c>
     </row>
     <row r="20" spans="1:8" x14ac:dyDescent="0.2">
@@ -1467,13 +1494,13 @@
         <v>22</v>
       </c>
       <c r="F20" t="s">
-        <v>67</v>
+        <v>62</v>
       </c>
       <c r="G20" t="s">
-        <v>103</v>
+        <v>104</v>
       </c>
       <c r="H20" s="2" t="s">
-        <v>66</v>
+        <v>61</v>
       </c>
     </row>
     <row r="21" spans="1:8" x14ac:dyDescent="0.2">
@@ -1481,7 +1508,7 @@
         <v>7</v>
       </c>
       <c r="B21" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="C21" t="s">
         <v>108</v>
@@ -1490,13 +1517,13 @@
         <v>22</v>
       </c>
       <c r="F21" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="G21" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="H21" s="2" t="s">
-        <v>68</v>
+        <v>63</v>
       </c>
     </row>
     <row r="22" spans="1:8" x14ac:dyDescent="0.2">
@@ -1504,7 +1531,7 @@
         <v>7</v>
       </c>
       <c r="B22" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C22" t="s">
         <v>108</v>
@@ -1513,13 +1540,13 @@
         <v>22</v>
       </c>
       <c r="F22" t="s">
-        <v>71</v>
+        <v>67</v>
       </c>
       <c r="G22" t="s">
-        <v>69</v>
+        <v>103</v>
       </c>
       <c r="H22" s="2" t="s">
-        <v>72</v>
+        <v>66</v>
       </c>
     </row>
     <row r="23" spans="1:8" x14ac:dyDescent="0.2">
@@ -1533,16 +1560,16 @@
         <v>108</v>
       </c>
       <c r="D23" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="F23" t="s">
-        <v>74</v>
+        <v>70</v>
       </c>
       <c r="G23" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H23" s="2" t="s">
-        <v>75</v>
+        <v>68</v>
       </c>
     </row>
     <row r="24" spans="1:8" x14ac:dyDescent="0.2">
@@ -1550,22 +1577,22 @@
         <v>7</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>14</v>
       </c>
       <c r="C24" t="s">
         <v>108</v>
       </c>
       <c r="D24" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F24" t="s">
-        <v>78</v>
+        <v>71</v>
       </c>
       <c r="G24" t="s">
-        <v>73</v>
+        <v>69</v>
       </c>
       <c r="H24" s="2" t="s">
-        <v>77</v>
+        <v>72</v>
       </c>
     </row>
     <row r="25" spans="1:8" x14ac:dyDescent="0.2">
@@ -1573,27 +1600,27 @@
         <v>7</v>
       </c>
       <c r="B25" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
         <v>108</v>
       </c>
       <c r="D25" t="s">
-        <v>22</v>
+        <v>76</v>
       </c>
       <c r="F25" t="s">
-        <v>79</v>
+        <v>74</v>
       </c>
       <c r="G25" t="s">
-        <v>65</v>
+        <v>73</v>
       </c>
       <c r="H25" s="2" t="s">
-        <v>80</v>
+        <v>75</v>
       </c>
     </row>
     <row r="26" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B26" t="s">
         <v>26</v>
@@ -1602,91 +1629,85 @@
         <v>108</v>
       </c>
       <c r="D26" t="s">
-        <v>76</v>
+        <v>6</v>
       </c>
       <c r="F26" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
       <c r="G26" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="H26" s="2" t="s">
-        <v>83</v>
+        <v>77</v>
       </c>
     </row>
     <row r="27" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
-        <v>8</v>
+        <v>7</v>
       </c>
       <c r="B27" t="s">
-        <v>26</v>
+        <v>106</v>
       </c>
       <c r="C27" t="s">
         <v>108</v>
       </c>
       <c r="D27" t="s">
-        <v>76</v>
+        <v>22</v>
       </c>
       <c r="F27" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="G27" t="s">
-        <v>85</v>
+        <v>65</v>
       </c>
       <c r="H27" s="2" t="s">
-        <v>86</v>
+        <v>80</v>
       </c>
     </row>
     <row r="28" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B28" t="s">
         <v>26</v>
       </c>
       <c r="C28" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D28" t="s">
-        <v>87</v>
-      </c>
-      <c r="E28" t="s">
-        <v>88</v>
+        <v>76</v>
       </c>
       <c r="F28" t="s">
-        <v>88</v>
+        <v>81</v>
       </c>
       <c r="G28" t="s">
-        <v>54</v>
+        <v>82</v>
       </c>
       <c r="H28" s="2" t="s">
-        <v>89</v>
+        <v>83</v>
       </c>
     </row>
     <row r="29" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
-        <v>7</v>
+        <v>8</v>
       </c>
       <c r="B29" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="C29" t="s">
         <v>108</v>
       </c>
       <c r="D29" t="s">
-        <v>22</v>
-      </c>
-      <c r="E29" t="s">
-        <v>94</v>
+        <v>76</v>
       </c>
       <c r="F29" t="s">
-        <v>90</v>
+        <v>84</v>
       </c>
       <c r="G29" t="s">
-        <v>91</v>
+        <v>85</v>
       </c>
       <c r="H29" s="2" t="s">
-        <v>92</v>
+        <v>86</v>
       </c>
     </row>
     <row r="30" spans="1:8" x14ac:dyDescent="0.2">
@@ -1694,25 +1715,25 @@
         <v>7</v>
       </c>
       <c r="B30" t="s">
-        <v>106</v>
+        <v>26</v>
       </c>
       <c r="C30" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D30" t="s">
-        <v>22</v>
+        <v>87</v>
       </c>
       <c r="E30" t="s">
-        <v>96</v>
+        <v>88</v>
       </c>
       <c r="F30" t="s">
-        <v>95</v>
+        <v>88</v>
       </c>
       <c r="G30" t="s">
-        <v>51</v>
+        <v>54</v>
       </c>
       <c r="H30" s="2" t="s">
-        <v>97</v>
+        <v>89</v>
       </c>
     </row>
     <row r="31" spans="1:8" x14ac:dyDescent="0.2">
@@ -1720,22 +1741,25 @@
         <v>7</v>
       </c>
       <c r="B31" t="s">
-        <v>101</v>
+        <v>106</v>
       </c>
       <c r="C31" t="s">
         <v>108</v>
       </c>
       <c r="D31" t="s">
-        <v>6</v>
+        <v>22</v>
+      </c>
+      <c r="E31" t="s">
+        <v>94</v>
       </c>
       <c r="F31" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="G31" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="H31" s="2" t="s">
-        <v>98</v>
+        <v>92</v>
       </c>
     </row>
     <row r="32" spans="1:8" x14ac:dyDescent="0.2">
@@ -1743,22 +1767,25 @@
         <v>7</v>
       </c>
       <c r="B32" t="s">
-        <v>9</v>
+        <v>106</v>
       </c>
       <c r="C32" t="s">
         <v>108</v>
       </c>
       <c r="D32" t="s">
-        <v>120</v>
+        <v>22</v>
+      </c>
+      <c r="E32" t="s">
+        <v>96</v>
       </c>
       <c r="F32" t="s">
-        <v>110</v>
+        <v>95</v>
       </c>
       <c r="G32" t="s">
-        <v>112</v>
+        <v>51</v>
       </c>
       <c r="H32" s="2" t="s">
-        <v>111</v>
+        <v>97</v>
       </c>
     </row>
     <row r="33" spans="1:8" x14ac:dyDescent="0.2">
@@ -1766,22 +1793,22 @@
         <v>7</v>
       </c>
       <c r="B33" t="s">
-        <v>115</v>
+        <v>101</v>
       </c>
       <c r="C33" t="s">
         <v>108</v>
       </c>
       <c r="D33" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="F33" t="s">
-        <v>113</v>
+        <v>99</v>
       </c>
       <c r="G33" t="s">
-        <v>112</v>
+        <v>100</v>
       </c>
       <c r="H33" s="2" t="s">
-        <v>114</v>
+        <v>98</v>
       </c>
     </row>
     <row r="34" spans="1:8" x14ac:dyDescent="0.2">
@@ -1789,7 +1816,7 @@
         <v>7</v>
       </c>
       <c r="B34" t="s">
-        <v>119</v>
+        <v>9</v>
       </c>
       <c r="C34" t="s">
         <v>108</v>
@@ -1798,13 +1825,13 @@
         <v>120</v>
       </c>
       <c r="F34" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="G34" t="s">
-        <v>118</v>
+        <v>112</v>
       </c>
       <c r="H34" s="2" t="s">
-        <v>116</v>
+        <v>111</v>
       </c>
     </row>
     <row r="35" spans="1:8" x14ac:dyDescent="0.2">
@@ -1812,22 +1839,22 @@
         <v>7</v>
       </c>
       <c r="B35" t="s">
-        <v>106</v>
+        <v>115</v>
       </c>
       <c r="C35" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D35" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="F35" t="s">
-        <v>126</v>
+        <v>113</v>
       </c>
       <c r="G35" t="s">
-        <v>124</v>
+        <v>112</v>
       </c>
       <c r="H35" s="2" t="s">
-        <v>125</v>
+        <v>114</v>
       </c>
     </row>
     <row r="36" spans="1:8" x14ac:dyDescent="0.2">
@@ -1835,22 +1862,22 @@
         <v>7</v>
       </c>
       <c r="B36" t="s">
-        <v>26</v>
+        <v>119</v>
       </c>
       <c r="C36" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D36" t="s">
-        <v>22</v>
+        <v>120</v>
       </c>
       <c r="F36" t="s">
-        <v>128</v>
+        <v>117</v>
       </c>
       <c r="G36" t="s">
-        <v>20</v>
+        <v>118</v>
       </c>
       <c r="H36" s="2" t="s">
-        <v>127</v>
+        <v>116</v>
       </c>
     </row>
     <row r="37" spans="1:8" x14ac:dyDescent="0.2">
@@ -1858,7 +1885,7 @@
         <v>7</v>
       </c>
       <c r="B37" t="s">
-        <v>14</v>
+        <v>106</v>
       </c>
       <c r="C37" t="s">
         <v>122</v>
@@ -1867,13 +1894,13 @@
         <v>22</v>
       </c>
       <c r="F37" t="s">
-        <v>130</v>
+        <v>126</v>
       </c>
       <c r="G37" t="s">
         <v>124</v>
       </c>
       <c r="H37" s="2" t="s">
-        <v>129</v>
+        <v>125</v>
       </c>
     </row>
     <row r="38" spans="1:8" x14ac:dyDescent="0.2">
@@ -1881,22 +1908,22 @@
         <v>7</v>
       </c>
       <c r="B38" t="s">
-        <v>14</v>
+        <v>26</v>
       </c>
       <c r="C38" t="s">
         <v>122</v>
       </c>
       <c r="D38" t="s">
-        <v>6</v>
+        <v>22</v>
       </c>
       <c r="F38" t="s">
-        <v>132</v>
+        <v>128</v>
       </c>
       <c r="G38" t="s">
-        <v>29</v>
+        <v>20</v>
       </c>
       <c r="H38" s="2" t="s">
-        <v>131</v>
+        <v>127</v>
       </c>
     </row>
     <row r="39" spans="1:8" x14ac:dyDescent="0.2">
@@ -1904,22 +1931,22 @@
         <v>7</v>
       </c>
       <c r="B39" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="C39" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D39" t="s">
-        <v>120</v>
+        <v>22</v>
       </c>
       <c r="F39" t="s">
-        <v>133</v>
+        <v>130</v>
       </c>
       <c r="G39" t="s">
-        <v>139</v>
+        <v>124</v>
       </c>
       <c r="H39" s="2" t="s">
-        <v>134</v>
+        <v>129</v>
       </c>
     </row>
     <row r="40" spans="1:8" x14ac:dyDescent="0.2">
@@ -1927,22 +1954,22 @@
         <v>7</v>
       </c>
       <c r="B40" t="s">
-        <v>121</v>
+        <v>14</v>
       </c>
       <c r="C40" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D40" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="F40" t="s">
-        <v>137</v>
+        <v>132</v>
       </c>
       <c r="G40" t="s">
-        <v>139</v>
+        <v>29</v>
       </c>
       <c r="H40" s="2" t="s">
-        <v>135</v>
+        <v>131</v>
       </c>
     </row>
     <row r="41" spans="1:8" x14ac:dyDescent="0.2">
@@ -1959,13 +1986,13 @@
         <v>120</v>
       </c>
       <c r="F41" t="s">
-        <v>138</v>
+        <v>133</v>
       </c>
       <c r="G41" t="s">
         <v>139</v>
       </c>
       <c r="H41" s="2" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
     </row>
     <row r="42" spans="1:8" x14ac:dyDescent="0.2">
@@ -1973,22 +2000,22 @@
         <v>7</v>
       </c>
       <c r="B42" t="s">
-        <v>26</v>
+        <v>121</v>
       </c>
       <c r="C42" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D42" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="F42" t="s">
-        <v>142</v>
+        <v>137</v>
       </c>
       <c r="G42" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="H42" s="2" t="s">
-        <v>140</v>
+        <v>135</v>
       </c>
     </row>
     <row r="43" spans="1:8" x14ac:dyDescent="0.2">
@@ -1996,22 +2023,22 @@
         <v>7</v>
       </c>
       <c r="B43" t="s">
-        <v>146</v>
+        <v>121</v>
       </c>
       <c r="C43" t="s">
-        <v>122</v>
+        <v>108</v>
       </c>
       <c r="D43" t="s">
-        <v>6</v>
+        <v>120</v>
       </c>
       <c r="F43" t="s">
-        <v>145</v>
+        <v>138</v>
       </c>
       <c r="G43" t="s">
-        <v>144</v>
+        <v>139</v>
       </c>
       <c r="H43" s="2" t="s">
-        <v>143</v>
+        <v>136</v>
       </c>
     </row>
     <row r="44" spans="1:8" x14ac:dyDescent="0.2">
@@ -2019,22 +2046,22 @@
         <v>7</v>
       </c>
       <c r="B44" t="s">
-        <v>9</v>
+        <v>26</v>
       </c>
       <c r="C44" t="s">
-        <v>108</v>
+        <v>122</v>
       </c>
       <c r="D44" t="s">
-        <v>120</v>
+        <v>6</v>
       </c>
       <c r="F44" t="s">
-        <v>194</v>
+        <v>142</v>
       </c>
       <c r="G44" t="s">
-        <v>196</v>
+        <v>141</v>
       </c>
       <c r="H44" s="2" t="s">
-        <v>195</v>
+        <v>140</v>
       </c>
     </row>
     <row r="45" spans="1:8" x14ac:dyDescent="0.2">
@@ -2042,70 +2069,118 @@
         <v>7</v>
       </c>
       <c r="B45" t="s">
+        <v>146</v>
+      </c>
+      <c r="C45" t="s">
+        <v>122</v>
+      </c>
+      <c r="D45" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" t="s">
+        <v>145</v>
+      </c>
+      <c r="G45" t="s">
+        <v>144</v>
+      </c>
+      <c r="H45" s="2" t="s">
+        <v>143</v>
+      </c>
+    </row>
+    <row r="46" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>7</v>
+      </c>
+      <c r="B46" t="s">
+        <v>9</v>
+      </c>
+      <c r="C46" t="s">
+        <v>108</v>
+      </c>
+      <c r="D46" t="s">
+        <v>120</v>
+      </c>
+      <c r="F46" t="s">
+        <v>194</v>
+      </c>
+      <c r="G46" t="s">
+        <v>196</v>
+      </c>
+      <c r="H46" s="2" t="s">
+        <v>195</v>
+      </c>
+    </row>
+    <row r="47" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
+        <v>7</v>
+      </c>
+      <c r="B47" t="s">
         <v>115</v>
       </c>
-      <c r="C45" t="s">
-        <v>108</v>
-      </c>
-      <c r="D45" t="s">
+      <c r="C47" t="s">
+        <v>108</v>
+      </c>
+      <c r="D47" t="s">
         <v>120</v>
       </c>
-      <c r="F45" t="s">
+      <c r="F47" t="s">
         <v>198</v>
       </c>
-      <c r="G45" t="s">
+      <c r="G47" t="s">
         <v>196</v>
       </c>
-      <c r="H45" s="2" t="s">
+      <c r="H47" s="2" t="s">
         <v>199</v>
       </c>
     </row>
   </sheetData>
   <hyperlinks>
-    <hyperlink ref="H6" r:id="rId1" xr:uid="{8BCE945E-B7AF-EE49-8DCF-6E4891E12673}"/>
-    <hyperlink ref="H2" r:id="rId2" xr:uid="{7A13AC78-F74E-3245-B3E1-C22974D223A8}"/>
-    <hyperlink ref="H4" r:id="rId3" xr:uid="{EFACDD5A-52B8-9B41-A329-7FDEB49D46A1}"/>
-    <hyperlink ref="H5" r:id="rId4" xr:uid="{5E1961D8-BCFA-5A4B-B0CE-9AE6016878E8}"/>
-    <hyperlink ref="H7" r:id="rId5" xr:uid="{41319DFA-9DFC-0447-9758-15770F7E5CD6}"/>
-    <hyperlink ref="H9" r:id="rId6" xr:uid="{25D4083B-8114-9A4F-8D20-800BBC727D0B}"/>
-    <hyperlink ref="H10" r:id="rId7" xr:uid="{83576F22-0B1C-1C4E-BA4B-D7BEE66F2AC6}"/>
-    <hyperlink ref="H8" r:id="rId8" xr:uid="{1541EB06-8DA9-1047-A2EA-9692DF4110C7}"/>
-    <hyperlink ref="H11" r:id="rId9" xr:uid="{A6BC24D6-D3E6-FC42-9621-15F6F0B6308B}"/>
-    <hyperlink ref="H12" r:id="rId10" xr:uid="{B4F5B5FB-9BDF-FE4B-B3D3-8F93FECC2FB0}"/>
-    <hyperlink ref="H3" r:id="rId11" xr:uid="{42138D86-981B-8642-93E4-E8FAF4D78555}"/>
-    <hyperlink ref="H13" r:id="rId12" display="https://www.amazon.co.uk/Machine-Learning-techniques-predictive-modeling-ebook/dp/B0114P1K1C/ref=pd_cp_351_1?_encoding=UTF8&amp;pd_rd_i=B0114P1K1C&amp;pd_rd_r=af4fbfc0-95ad-11e8-9889-7529903ded07&amp;pd_rd_w=zF0PO&amp;pd_rd_wg=CGjia&amp;pf_rd_i=desktop-dp-sims&amp;pf_rd_m=A3P5ROKL5A1OLE&amp;pf_rd_p=3262852920272843952&amp;pf_rd_r=TA0Z2YJAZ5TNV4SCTFN7&amp;pf_rd_s=desktop-dp-sims&amp;pf_rd_t=40701&amp;psc=1&amp;refRID=TA0Z2YJAZ5TNV4SCTFN7" xr:uid="{0EBAF09C-EDEB-9942-A271-1E2C2C8DC8B0}"/>
-    <hyperlink ref="H14" r:id="rId13" xr:uid="{0EA9A260-79CC-7043-9383-13611CE429EB}"/>
-    <hyperlink ref="H15" r:id="rId14" xr:uid="{FB92CED3-CF5F-2245-9DFC-BBC6795117C9}"/>
-    <hyperlink ref="H16" r:id="rId15" xr:uid="{A3B2E084-8CDC-6B43-ACFF-08484645A4A6}"/>
-    <hyperlink ref="H17" r:id="rId16" xr:uid="{E45D6CBC-F840-6641-AB27-12B2D131F0AC}"/>
-    <hyperlink ref="H18" r:id="rId17" xr:uid="{1325A89E-381A-9B4D-A157-DFE892F67472}"/>
-    <hyperlink ref="H19" r:id="rId18" xr:uid="{D2FF1E86-B581-6F48-B526-86D92179D78A}"/>
-    <hyperlink ref="H20" r:id="rId19" xr:uid="{19992164-4EBA-1E4E-BE6D-A148392A3DC4}"/>
-    <hyperlink ref="H21" r:id="rId20" xr:uid="{FCFC098A-9B88-2142-9037-CCD738A501C5}"/>
-    <hyperlink ref="H22" r:id="rId21" xr:uid="{0970DA55-6AE0-2D40-8B9E-57C33DCD7218}"/>
-    <hyperlink ref="H23" r:id="rId22" xr:uid="{751B9D75-6058-CE4B-A9C7-8188075AD9ED}"/>
-    <hyperlink ref="H24" r:id="rId23" xr:uid="{FCBEF050-2E0C-0440-97AD-E81E658BF256}"/>
-    <hyperlink ref="H25" r:id="rId24" xr:uid="{52FEB207-99D8-0D49-989A-11DFEFCDC854}"/>
-    <hyperlink ref="H26" r:id="rId25" xr:uid="{B5EF3B4C-B5CD-C142-BD00-B72BB9E05209}"/>
-    <hyperlink ref="H27" r:id="rId26" xr:uid="{EF89A846-EAC7-E742-B324-C907BDD890E7}"/>
-    <hyperlink ref="H28" r:id="rId27" xr:uid="{A0403370-5B58-F84D-9D96-BFFA80790A0C}"/>
-    <hyperlink ref="H29" r:id="rId28" xr:uid="{F1826E6B-0AC0-1D4B-BF88-0562D80BF096}"/>
-    <hyperlink ref="H30" r:id="rId29" xr:uid="{4B5DDB02-2A74-D54D-B0D2-12010C30CB24}"/>
-    <hyperlink ref="H31" r:id="rId30" xr:uid="{2DDD426F-9C96-EE46-BB82-2E341B75538F}"/>
-    <hyperlink ref="H32" r:id="rId31" xr:uid="{37FC97B4-BB6A-0946-8BAF-6E70A1546C22}"/>
-    <hyperlink ref="H33" r:id="rId32" xr:uid="{0EDFF259-7500-084A-9EAC-B051E9D2DA79}"/>
-    <hyperlink ref="H34" r:id="rId33" xr:uid="{89B3F55D-4B03-A14F-B123-7E0A4E3519F7}"/>
-    <hyperlink ref="H35" r:id="rId34" xr:uid="{5BA90A56-1AF0-A440-B86D-DB8E6EEBB181}"/>
-    <hyperlink ref="H36" r:id="rId35" xr:uid="{D558C84B-B451-194F-911F-61CDF46476FE}"/>
-    <hyperlink ref="H37" r:id="rId36" xr:uid="{1DB450E6-84B1-B841-A5BC-63A0C5628305}"/>
-    <hyperlink ref="H38" r:id="rId37" xr:uid="{1690FCF9-A247-1B42-9AA7-6ABA716E1F98}"/>
-    <hyperlink ref="H39" r:id="rId38" xr:uid="{61F33400-0938-5840-8462-355E3BDC6D36}"/>
-    <hyperlink ref="H40" r:id="rId39" xr:uid="{22BF016A-F61B-2441-A2D7-8C5C7B8A1CCC}"/>
-    <hyperlink ref="H41" r:id="rId40" xr:uid="{9E383B6C-6E2B-0B4A-9920-A2A2592A4E93}"/>
-    <hyperlink ref="H42" r:id="rId41" xr:uid="{AEAC8E0D-36A7-F74C-9A98-3F00555A6C56}"/>
-    <hyperlink ref="H43" r:id="rId42" xr:uid="{EA1B315E-C585-884A-9D4B-458B01F703F0}"/>
-    <hyperlink ref="H44" r:id="rId43" xr:uid="{69BD5659-0F20-614B-9C4F-3A61021D6A98}"/>
-    <hyperlink ref="H45" r:id="rId44" xr:uid="{9E13235A-1E25-8145-BE2D-EA8A78F0F883}"/>
+    <hyperlink ref="H8" r:id="rId1" xr:uid="{8BCE945E-B7AF-EE49-8DCF-6E4891E12673}"/>
+    <hyperlink ref="H4" r:id="rId2" xr:uid="{7A13AC78-F74E-3245-B3E1-C22974D223A8}"/>
+    <hyperlink ref="H6" r:id="rId3" xr:uid="{EFACDD5A-52B8-9B41-A329-7FDEB49D46A1}"/>
+    <hyperlink ref="H7" r:id="rId4" xr:uid="{5E1961D8-BCFA-5A4B-B0CE-9AE6016878E8}"/>
+    <hyperlink ref="H9" r:id="rId5" xr:uid="{41319DFA-9DFC-0447-9758-15770F7E5CD6}"/>
+    <hyperlink ref="H11" r:id="rId6" xr:uid="{25D4083B-8114-9A4F-8D20-800BBC727D0B}"/>
+    <hyperlink ref="H12" r:id="rId7" xr:uid="{83576F22-0B1C-1C4E-BA4B-D7BEE66F2AC6}"/>
+    <hyperlink ref="H10" r:id="rId8" xr:uid="{1541EB06-8DA9-1047-A2EA-9692DF4110C7}"/>
+    <hyperlink ref="H13" r:id="rId9" xr:uid="{A6BC24D6-D3E6-FC42-9621-15F6F0B6308B}"/>
+    <hyperlink ref="H14" r:id="rId10" xr:uid="{B4F5B5FB-9BDF-FE4B-B3D3-8F93FECC2FB0}"/>
+    <hyperlink ref="H5" r:id="rId11" xr:uid="{42138D86-981B-8642-93E4-E8FAF4D78555}"/>
+    <hyperlink ref="H15" r:id="rId12" display="https://www.amazon.co.uk/Machine-Learning-techniques-predictive-modeling-ebook/dp/B0114P1K1C/ref=pd_cp_351_1?_encoding=UTF8&amp;pd_rd_i=B0114P1K1C&amp;pd_rd_r=af4fbfc0-95ad-11e8-9889-7529903ded07&amp;pd_rd_w=zF0PO&amp;pd_rd_wg=CGjia&amp;pf_rd_i=desktop-dp-sims&amp;pf_rd_m=A3P5ROKL5A1OLE&amp;pf_rd_p=3262852920272843952&amp;pf_rd_r=TA0Z2YJAZ5TNV4SCTFN7&amp;pf_rd_s=desktop-dp-sims&amp;pf_rd_t=40701&amp;psc=1&amp;refRID=TA0Z2YJAZ5TNV4SCTFN7" xr:uid="{0EBAF09C-EDEB-9942-A271-1E2C2C8DC8B0}"/>
+    <hyperlink ref="H16" r:id="rId13" xr:uid="{0EA9A260-79CC-7043-9383-13611CE429EB}"/>
+    <hyperlink ref="H17" r:id="rId14" xr:uid="{FB92CED3-CF5F-2245-9DFC-BBC6795117C9}"/>
+    <hyperlink ref="H18" r:id="rId15" xr:uid="{A3B2E084-8CDC-6B43-ACFF-08484645A4A6}"/>
+    <hyperlink ref="H19" r:id="rId16" xr:uid="{E45D6CBC-F840-6641-AB27-12B2D131F0AC}"/>
+    <hyperlink ref="H20" r:id="rId17" xr:uid="{1325A89E-381A-9B4D-A157-DFE892F67472}"/>
+    <hyperlink ref="H21" r:id="rId18" xr:uid="{D2FF1E86-B581-6F48-B526-86D92179D78A}"/>
+    <hyperlink ref="H22" r:id="rId19" xr:uid="{19992164-4EBA-1E4E-BE6D-A148392A3DC4}"/>
+    <hyperlink ref="H23" r:id="rId20" xr:uid="{FCFC098A-9B88-2142-9037-CCD738A501C5}"/>
+    <hyperlink ref="H24" r:id="rId21" xr:uid="{0970DA55-6AE0-2D40-8B9E-57C33DCD7218}"/>
+    <hyperlink ref="H25" r:id="rId22" xr:uid="{751B9D75-6058-CE4B-A9C7-8188075AD9ED}"/>
+    <hyperlink ref="H26" r:id="rId23" xr:uid="{FCBEF050-2E0C-0440-97AD-E81E658BF256}"/>
+    <hyperlink ref="H27" r:id="rId24" xr:uid="{52FEB207-99D8-0D49-989A-11DFEFCDC854}"/>
+    <hyperlink ref="H28" r:id="rId25" xr:uid="{B5EF3B4C-B5CD-C142-BD00-B72BB9E05209}"/>
+    <hyperlink ref="H29" r:id="rId26" xr:uid="{EF89A846-EAC7-E742-B324-C907BDD890E7}"/>
+    <hyperlink ref="H30" r:id="rId27" xr:uid="{A0403370-5B58-F84D-9D96-BFFA80790A0C}"/>
+    <hyperlink ref="H31" r:id="rId28" xr:uid="{F1826E6B-0AC0-1D4B-BF88-0562D80BF096}"/>
+    <hyperlink ref="H32" r:id="rId29" xr:uid="{4B5DDB02-2A74-D54D-B0D2-12010C30CB24}"/>
+    <hyperlink ref="H33" r:id="rId30" xr:uid="{2DDD426F-9C96-EE46-BB82-2E341B75538F}"/>
+    <hyperlink ref="H34" r:id="rId31" xr:uid="{37FC97B4-BB6A-0946-8BAF-6E70A1546C22}"/>
+    <hyperlink ref="H35" r:id="rId32" xr:uid="{0EDFF259-7500-084A-9EAC-B051E9D2DA79}"/>
+    <hyperlink ref="H36" r:id="rId33" xr:uid="{89B3F55D-4B03-A14F-B123-7E0A4E3519F7}"/>
+    <hyperlink ref="H37" r:id="rId34" xr:uid="{5BA90A56-1AF0-A440-B86D-DB8E6EEBB181}"/>
+    <hyperlink ref="H38" r:id="rId35" xr:uid="{D558C84B-B451-194F-911F-61CDF46476FE}"/>
+    <hyperlink ref="H39" r:id="rId36" xr:uid="{1DB450E6-84B1-B841-A5BC-63A0C5628305}"/>
+    <hyperlink ref="H40" r:id="rId37" xr:uid="{1690FCF9-A247-1B42-9AA7-6ABA716E1F98}"/>
+    <hyperlink ref="H41" r:id="rId38" xr:uid="{61F33400-0938-5840-8462-355E3BDC6D36}"/>
+    <hyperlink ref="H42" r:id="rId39" xr:uid="{22BF016A-F61B-2441-A2D7-8C5C7B8A1CCC}"/>
+    <hyperlink ref="H43" r:id="rId40" xr:uid="{9E383B6C-6E2B-0B4A-9920-A2A2592A4E93}"/>
+    <hyperlink ref="H44" r:id="rId41" xr:uid="{AEAC8E0D-36A7-F74C-9A98-3F00555A6C56}"/>
+    <hyperlink ref="H45" r:id="rId42" xr:uid="{EA1B315E-C585-884A-9D4B-458B01F703F0}"/>
+    <hyperlink ref="H46" r:id="rId43" xr:uid="{69BD5659-0F20-614B-9C4F-3A61021D6A98}"/>
+    <hyperlink ref="H47" r:id="rId44" xr:uid="{9E13235A-1E25-8145-BE2D-EA8A78F0F883}"/>
+    <hyperlink ref="H2" r:id="rId45" xr:uid="{50849457-6E21-9C4A-96D1-B1F95680A3AA}"/>
+    <hyperlink ref="H3" r:id="rId46" xr:uid="{355E11C0-6E21-7044-976B-6E0BCE391452}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2114,10 +2189,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6A4CF0-E7B1-A149-8123-B7914F3BFAC3}">
-  <dimension ref="A1:B34"/>
+  <dimension ref="A1:B37"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="A34" sqref="A34"/>
+      <selection activeCell="B38" sqref="B38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2398,9 +2473,34 @@
         <v>197</v>
       </c>
     </row>
+    <row r="35" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A35" t="s">
+        <v>204</v>
+      </c>
+      <c r="B35" t="s">
+        <v>203</v>
+      </c>
+    </row>
+    <row r="36" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A36" t="s">
+        <v>206</v>
+      </c>
+      <c r="B36" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="37" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A37" t="s">
+        <v>207</v>
+      </c>
+      <c r="B37" s="2" t="s">
+        <v>208</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B34" r:id="rId1" xr:uid="{EB0E88FC-9F49-F04E-BD45-78B47D7913D3}"/>
+    <hyperlink ref="B37" r:id="rId2" xr:uid="{D8323E4A-B831-2941-80C6-178A1FFF79FB}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>

<commit_message>
Updating Resources page to latest API changes + adding in additional resources, including GIT and probability
</commit_message>
<xml_diff>
--- a/Resources.xlsx
+++ b/Resources.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10414"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10209"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/gerhardgroenewald/Documents/R Projects/gerhardgroenewald.co.uk/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AAE5C90-7616-AF4C-A731-92251FD46DFC}" xr6:coauthVersionLast="43" xr6:coauthVersionMax="43" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCB17DDF-D761-884C-85F9-EC86CEAA2D34}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="38400" windowHeight="21600" xr2:uid="{D09C6361-AE78-2141-8FAE-67D4DAF24799}"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="38400" windowHeight="21600" xr2:uid="{D09C6361-AE78-2141-8FAE-67D4DAF24799}"/>
   </bookViews>
   <sheets>
     <sheet name="Resources" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="412" uniqueCount="209">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="437" uniqueCount="223">
   <si>
     <t>Source</t>
   </si>
@@ -654,6 +654,48 @@
   </si>
   <si>
     <t>https://www.geographie.uni-jena.de/en/Muenchow.html</t>
+  </si>
+  <si>
+    <t>Interpretable Machine Learning  A Guide for Making Black Box Models Explainable.</t>
+  </si>
+  <si>
+    <t>Christoph Molnar</t>
+  </si>
+  <si>
+    <t>https://christophm.github.io</t>
+  </si>
+  <si>
+    <t>https://christophm.github.io/interpretable-ml-book/</t>
+  </si>
+  <si>
+    <t>Python, Statistics</t>
+  </si>
+  <si>
+    <t>https://machinelearningmastery.com/probability-for-machine-learning/</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Probability for Machine Learning </t>
+  </si>
+  <si>
+    <t>Probability, Programming, Model</t>
+  </si>
+  <si>
+    <t>Reference, Training</t>
+  </si>
+  <si>
+    <t>GIT</t>
+  </si>
+  <si>
+    <t>Atlassian</t>
+  </si>
+  <si>
+    <t>Learn Git with Bitbucket Cloud</t>
+  </si>
+  <si>
+    <t>https://www.atlassian.com/git</t>
+  </si>
+  <si>
+    <t>https://www.atlassian.com/</t>
   </si>
 </sst>
 </file>
@@ -1019,10 +1061,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{275A2A9A-7374-FC4C-AFC4-53788431EF74}">
-  <dimension ref="A1:I47"/>
+  <dimension ref="A1:I50"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="129" workbookViewId="0">
-      <selection activeCell="C3" sqref="C3:H3"/>
+    <sheetView tabSelected="1" topLeftCell="A39" zoomScale="129" workbookViewId="0">
+      <selection activeCell="F50" sqref="F50"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2131,6 +2173,75 @@
       </c>
       <c r="H47" s="2" t="s">
         <v>199</v>
+      </c>
+    </row>
+    <row r="48" spans="1:8" ht="51" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
+        <v>7</v>
+      </c>
+      <c r="B48" t="s">
+        <v>106</v>
+      </c>
+      <c r="C48" t="s">
+        <v>122</v>
+      </c>
+      <c r="D48" t="s">
+        <v>120</v>
+      </c>
+      <c r="F48" s="1" t="s">
+        <v>209</v>
+      </c>
+      <c r="G48" t="s">
+        <v>210</v>
+      </c>
+      <c r="H48" s="2" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="49" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A49" t="s">
+        <v>45</v>
+      </c>
+      <c r="B49" t="s">
+        <v>216</v>
+      </c>
+      <c r="C49" t="s">
+        <v>217</v>
+      </c>
+      <c r="D49" t="s">
+        <v>213</v>
+      </c>
+      <c r="F49" t="s">
+        <v>215</v>
+      </c>
+      <c r="G49" t="s">
+        <v>47</v>
+      </c>
+      <c r="H49" s="2" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="50" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A50" t="s">
+        <v>7</v>
+      </c>
+      <c r="B50" t="s">
+        <v>26</v>
+      </c>
+      <c r="C50" t="s">
+        <v>108</v>
+      </c>
+      <c r="D50" t="s">
+        <v>218</v>
+      </c>
+      <c r="F50" t="s">
+        <v>220</v>
+      </c>
+      <c r="G50" t="s">
+        <v>219</v>
+      </c>
+      <c r="H50" s="2" t="s">
+        <v>221</v>
       </c>
     </row>
   </sheetData>
@@ -2181,6 +2292,9 @@
     <hyperlink ref="H47" r:id="rId44" xr:uid="{9E13235A-1E25-8145-BE2D-EA8A78F0F883}"/>
     <hyperlink ref="H2" r:id="rId45" xr:uid="{50849457-6E21-9C4A-96D1-B1F95680A3AA}"/>
     <hyperlink ref="H3" r:id="rId46" xr:uid="{355E11C0-6E21-7044-976B-6E0BCE391452}"/>
+    <hyperlink ref="H48" r:id="rId47" xr:uid="{CD683513-A6B1-CD4F-A167-CE3097EE4405}"/>
+    <hyperlink ref="H49" r:id="rId48" xr:uid="{4486003F-777B-EA4C-BF6B-9B2DCD429E39}"/>
+    <hyperlink ref="H50" r:id="rId49" xr:uid="{C66906A1-2C63-0D48-9400-A5464831586E}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup paperSize="9" orientation="portrait" horizontalDpi="0" verticalDpi="0"/>
@@ -2189,10 +2303,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{7F6A4CF0-E7B1-A149-8123-B7914F3BFAC3}">
-  <dimension ref="A1:B37"/>
+  <dimension ref="A1:B39"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="B38" sqref="B38"/>
+      <selection activeCell="A40" sqref="A40"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2497,10 +2611,28 @@
         <v>208</v>
       </c>
     </row>
+    <row r="38" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A38" t="s">
+        <v>210</v>
+      </c>
+      <c r="B38" s="2" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="39" spans="1:2" x14ac:dyDescent="0.2">
+      <c r="A39" t="s">
+        <v>219</v>
+      </c>
+      <c r="B39" s="2" t="s">
+        <v>222</v>
+      </c>
+    </row>
   </sheetData>
   <hyperlinks>
     <hyperlink ref="B34" r:id="rId1" xr:uid="{EB0E88FC-9F49-F04E-BD45-78B47D7913D3}"/>
     <hyperlink ref="B37" r:id="rId2" xr:uid="{D8323E4A-B831-2941-80C6-178A1FFF79FB}"/>
+    <hyperlink ref="B38" r:id="rId3" xr:uid="{789D97DE-CBCA-0E4C-8BAE-7BF6BF128D86}"/>
+    <hyperlink ref="B39" r:id="rId4" xr:uid="{1D491FDB-2A2E-5445-9F5F-74E6D337CDC8}"/>
   </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>

</xml_diff>